<commit_message>
bugs represent Image et web adresse corrigés maj readme
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Name|type='string'</t>
   </si>
@@ -91,22 +91,34 @@
     <t>Pic|dlimage</t>
   </si>
   <si>
+    <t>Links|webaddr</t>
+  </si>
+  <si>
     <t>vuemphis</t>
   </si>
   <si>
-    <t>City1.png</t>
+    <t>City1.jpg</t>
+  </si>
+  <si>
+    <t>http://commitment.cornell.edu/</t>
   </si>
   <si>
     <t>comond</t>
   </si>
   <si>
-    <t>City2.png|River.png</t>
+    <t>City2.jpg|River.jpg</t>
+  </si>
+  <si>
+    <t>http://www.presidence.cg/accueil/</t>
   </si>
   <si>
     <t>breefburn</t>
   </si>
   <si>
-    <t>River.png</t>
+    <t>River.jpg</t>
+  </si>
+  <si>
+    <t>http://www.sydneydance.com.au/</t>
   </si>
   <si>
     <t>etreimouth</t>
@@ -263,7 +275,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -489,10 +501,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -512,16 +524,22 @@
       <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>200</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,10 +547,13 @@
         <v>201</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,10 +561,13 @@
         <v>202</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,7 +575,7 @@
         <v>203</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -560,7 +584,7 @@
         <v>204</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -569,7 +593,7 @@
         <v>205</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -578,7 +602,7 @@
         <v>220</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -587,7 +611,7 @@
         <v>254</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -596,7 +620,7 @@
         <v>270</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -605,11 +629,16 @@
         <v>320</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="http://commitment.cornell.edu/"/>
+    <hyperlink ref="D3" r:id="rId2" display="http://www.presidence.cg/accueil/"/>
+    <hyperlink ref="D4" r:id="rId3" display="http://www.sydneydance.com.au/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
clean code +renomme boo et doo en searchReferences et searchPics
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -276,16 +276,17 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.8979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="38.7857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>